<commit_message>
First merge for new sprites
</commit_message>
<xml_diff>
--- a/src/renderer/resources/db/sounds.xlsx
+++ b/src/renderer/resources/db/sounds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/comseong/dev/entry/entry-offline/src/renderer/resources/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E59D599-4728-874A-AE1B-9746AADE96E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D065DB29-6D2B-9A46-B357-E62208198F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3438,12 +3438,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -3452,28 +3467,28 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -3779,7 +3794,8 @@
   <dimension ref="A1:J226"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -3788,40 +3804,40 @@
     <col min="5" max="5" width="14.6640625" customWidth="1"/>
     <col min="6" max="6" width="27.5" customWidth="1"/>
     <col min="7" max="7" width="36.33203125" customWidth="1"/>
-    <col min="8" max="8" width="31" style="10" customWidth="1"/>
-    <col min="9" max="9" width="47" style="4" customWidth="1"/>
-    <col min="10" max="10" width="41.6640625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="31" style="5" customWidth="1"/>
+    <col min="9" max="9" width="47" style="1" customWidth="1"/>
+    <col min="10" max="10" width="41.6640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>747</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
         <v>748</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="10" t="s">
         <v>749</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="10" t="s">
         <v>750</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="10" t="s">
         <v>751</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="11" t="s">
         <v>752</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="11" t="s">
         <v>753</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="12" t="s">
         <v>754</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="13" t="s">
         <v>755</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="14" t="s">
         <v>1079</v>
       </c>
     </row>
@@ -3847,10 +3863,10 @@
       <c r="G2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3876,10 +3892,10 @@
       <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3905,10 +3921,10 @@
       <c r="G4" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3934,10 +3950,10 @@
       <c r="G5" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3963,10 +3979,10 @@
       <c r="G6" t="s">
         <v>1009</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="5" t="s">
         <v>1068</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="1" t="s">
         <v>1010</v>
       </c>
     </row>
@@ -3992,10 +4008,10 @@
       <c r="G7" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="1" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4021,10 +4037,10 @@
       <c r="G8" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="1" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4050,10 +4066,10 @@
       <c r="G9" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="1" t="s">
         <v>46</v>
       </c>
     </row>
@@ -4079,10 +4095,10 @@
       <c r="G10" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="1" t="s">
         <v>51</v>
       </c>
     </row>
@@ -4108,10 +4124,10 @@
       <c r="G11" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="1" t="s">
         <v>57</v>
       </c>
     </row>
@@ -4137,10 +4153,10 @@
       <c r="G12" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="1" t="s">
         <v>63</v>
       </c>
     </row>
@@ -4166,10 +4182,10 @@
       <c r="G13" t="s">
         <v>66</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="1" t="s">
         <v>68</v>
       </c>
     </row>
@@ -4195,10 +4211,10 @@
       <c r="G14" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="1" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4224,10 +4240,10 @@
       <c r="G15" t="s">
         <v>76</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="1" t="s">
         <v>77</v>
       </c>
     </row>
@@ -4253,10 +4269,10 @@
       <c r="G16" t="s">
         <v>80</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -4282,10 +4298,10 @@
       <c r="G17" t="s">
         <v>85</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="1" t="s">
         <v>87</v>
       </c>
     </row>
@@ -4311,10 +4327,10 @@
       <c r="G18" t="s">
         <v>90</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="1" t="s">
         <v>92</v>
       </c>
     </row>
@@ -4340,10 +4356,10 @@
       <c r="G19" t="s">
         <v>95</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="1" t="s">
         <v>97</v>
       </c>
     </row>
@@ -4369,10 +4385,10 @@
       <c r="G20" t="s">
         <v>100</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="I20" s="1" t="s">
         <v>102</v>
       </c>
     </row>
@@ -4398,10 +4414,10 @@
       <c r="G21" t="s">
         <v>105</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="H21" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="I21" s="4" t="s">
+      <c r="I21" s="1" t="s">
         <v>107</v>
       </c>
     </row>
@@ -4427,10 +4443,10 @@
       <c r="G22" t="s">
         <v>110</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="H22" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="I22" s="1" t="s">
         <v>112</v>
       </c>
     </row>
@@ -4456,10 +4472,10 @@
       <c r="G23" t="s">
         <v>115</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="H23" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="I23" s="1" t="s">
         <v>117</v>
       </c>
     </row>
@@ -4485,10 +4501,10 @@
       <c r="G24" t="s">
         <v>121</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="H24" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="I24" s="1" t="s">
         <v>123</v>
       </c>
     </row>
@@ -4514,10 +4530,10 @@
       <c r="G25" t="s">
         <v>126</v>
       </c>
-      <c r="H25" s="10" t="s">
+      <c r="H25" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="I25" s="4" t="s">
+      <c r="I25" s="1" t="s">
         <v>128</v>
       </c>
     </row>
@@ -4540,10 +4556,10 @@
       <c r="G26" t="s">
         <v>132</v>
       </c>
-      <c r="H26" s="10" t="s">
+      <c r="H26" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="I26" s="1" t="s">
         <v>134</v>
       </c>
     </row>
@@ -4569,10 +4585,10 @@
       <c r="G27" t="s">
         <v>137</v>
       </c>
-      <c r="H27" s="10" t="s">
+      <c r="H27" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="I27" s="1" t="s">
         <v>139</v>
       </c>
     </row>
@@ -4598,10 +4614,10 @@
       <c r="G28" t="s">
         <v>142</v>
       </c>
-      <c r="H28" s="10" t="s">
+      <c r="H28" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="I28" s="1" t="s">
         <v>144</v>
       </c>
     </row>
@@ -4627,10 +4643,10 @@
       <c r="G29" t="s">
         <v>148</v>
       </c>
-      <c r="H29" s="10" t="s">
+      <c r="H29" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="I29" s="4" t="s">
+      <c r="I29" s="1" t="s">
         <v>150</v>
       </c>
     </row>
@@ -4656,10 +4672,10 @@
       <c r="G30" t="s">
         <v>153</v>
       </c>
-      <c r="H30" s="10" t="s">
+      <c r="H30" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="I30" s="4" t="s">
+      <c r="I30" s="1" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4685,10 +4701,10 @@
       <c r="G31" t="s">
         <v>158</v>
       </c>
-      <c r="H31" s="10" t="s">
+      <c r="H31" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="I31" s="4" t="s">
+      <c r="I31" s="1" t="s">
         <v>160</v>
       </c>
     </row>
@@ -4714,10 +4730,10 @@
       <c r="G32" t="s">
         <v>163</v>
       </c>
-      <c r="H32" s="10" t="s">
+      <c r="H32" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="I32" s="1" t="s">
         <v>165</v>
       </c>
     </row>
@@ -4743,10 +4759,10 @@
       <c r="G33" t="s">
         <v>168</v>
       </c>
-      <c r="H33" s="10" t="s">
+      <c r="H33" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="I33" s="4" t="s">
+      <c r="I33" s="1" t="s">
         <v>170</v>
       </c>
     </row>
@@ -4772,10 +4788,10 @@
       <c r="G34" t="s">
         <v>173</v>
       </c>
-      <c r="H34" s="10" t="s">
+      <c r="H34" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="I34" s="4" t="s">
+      <c r="I34" s="1" t="s">
         <v>175</v>
       </c>
     </row>
@@ -4801,10 +4817,10 @@
       <c r="G35" t="s">
         <v>178</v>
       </c>
-      <c r="H35" s="10" t="s">
+      <c r="H35" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="I35" s="4" t="s">
+      <c r="I35" s="1" t="s">
         <v>180</v>
       </c>
     </row>
@@ -4830,10 +4846,10 @@
       <c r="G36" t="s">
         <v>183</v>
       </c>
-      <c r="H36" s="10" t="s">
+      <c r="H36" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="I36" s="4" t="s">
+      <c r="I36" s="1" t="s">
         <v>185</v>
       </c>
     </row>
@@ -4859,10 +4875,10 @@
       <c r="G37" t="s">
         <v>188</v>
       </c>
-      <c r="H37" s="10" t="s">
+      <c r="H37" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="I37" s="4" t="s">
+      <c r="I37" s="1" t="s">
         <v>190</v>
       </c>
     </row>
@@ -4888,10 +4904,10 @@
       <c r="G38" t="s">
         <v>193</v>
       </c>
-      <c r="H38" s="10" t="s">
+      <c r="H38" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="I38" s="4" t="s">
+      <c r="I38" s="1" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4917,10 +4933,10 @@
       <c r="G39" t="s">
         <v>198</v>
       </c>
-      <c r="H39" s="10" t="s">
+      <c r="H39" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="I39" s="4" t="s">
+      <c r="I39" s="1" t="s">
         <v>200</v>
       </c>
     </row>
@@ -4946,10 +4962,10 @@
       <c r="G40" t="s">
         <v>203</v>
       </c>
-      <c r="H40" s="10" t="s">
+      <c r="H40" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="I40" s="4" t="s">
+      <c r="I40" s="1" t="s">
         <v>205</v>
       </c>
     </row>
@@ -4975,10 +4991,10 @@
       <c r="G41" t="s">
         <v>1012</v>
       </c>
-      <c r="H41" s="10" t="s">
+      <c r="H41" s="5" t="s">
         <v>1013</v>
       </c>
-      <c r="I41" s="4" t="s">
+      <c r="I41" s="1" t="s">
         <v>1014</v>
       </c>
     </row>
@@ -5004,10 +5020,10 @@
       <c r="G42" t="s">
         <v>209</v>
       </c>
-      <c r="H42" s="10" t="s">
+      <c r="H42" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="I42" s="4" t="s">
+      <c r="I42" s="1" t="s">
         <v>211</v>
       </c>
     </row>
@@ -5030,10 +5046,10 @@
       <c r="G43" t="s">
         <v>214</v>
       </c>
-      <c r="H43" s="10" t="s">
+      <c r="H43" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="I43" s="4" t="s">
+      <c r="I43" s="1" t="s">
         <v>216</v>
       </c>
     </row>
@@ -5059,10 +5075,10 @@
       <c r="G44" t="s">
         <v>219</v>
       </c>
-      <c r="H44" s="10" t="s">
+      <c r="H44" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="I44" s="4" t="s">
+      <c r="I44" s="1" t="s">
         <v>221</v>
       </c>
     </row>
@@ -5088,10 +5104,10 @@
       <c r="G45" t="s">
         <v>224</v>
       </c>
-      <c r="H45" s="10" t="s">
+      <c r="H45" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="I45" s="4" t="s">
+      <c r="I45" s="1" t="s">
         <v>226</v>
       </c>
     </row>
@@ -5117,10 +5133,10 @@
       <c r="G46" t="s">
         <v>229</v>
       </c>
-      <c r="H46" s="10" t="s">
+      <c r="H46" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="I46" s="4" t="s">
+      <c r="I46" s="1" t="s">
         <v>231</v>
       </c>
     </row>
@@ -5143,10 +5159,10 @@
       <c r="G47" t="s">
         <v>234</v>
       </c>
-      <c r="H47" s="10" t="s">
+      <c r="H47" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="I47" s="4" t="s">
+      <c r="I47" s="1" t="s">
         <v>235</v>
       </c>
     </row>
@@ -5172,10 +5188,10 @@
       <c r="G48" t="s">
         <v>238</v>
       </c>
-      <c r="H48" s="10" t="s">
+      <c r="H48" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="I48" s="4" t="s">
+      <c r="I48" s="1" t="s">
         <v>240</v>
       </c>
     </row>
@@ -5201,10 +5217,10 @@
       <c r="G49" t="s">
         <v>244</v>
       </c>
-      <c r="H49" s="10" t="s">
+      <c r="H49" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="I49" s="4" t="s">
+      <c r="I49" s="1" t="s">
         <v>246</v>
       </c>
     </row>
@@ -5230,10 +5246,10 @@
       <c r="G50" t="s">
         <v>249</v>
       </c>
-      <c r="H50" s="10" t="s">
+      <c r="H50" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="I50" s="4" t="s">
+      <c r="I50" s="1" t="s">
         <v>250</v>
       </c>
     </row>
@@ -5259,10 +5275,10 @@
       <c r="G51" t="s">
         <v>253</v>
       </c>
-      <c r="H51" s="10" t="s">
+      <c r="H51" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="I51" s="4" t="s">
+      <c r="I51" s="1" t="s">
         <v>255</v>
       </c>
     </row>
@@ -5288,10 +5304,10 @@
       <c r="G52" t="s">
         <v>258</v>
       </c>
-      <c r="H52" s="10" t="s">
+      <c r="H52" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="I52" s="4" t="s">
+      <c r="I52" s="1" t="s">
         <v>260</v>
       </c>
     </row>
@@ -5317,10 +5333,10 @@
       <c r="G53" t="s">
         <v>263</v>
       </c>
-      <c r="H53" s="10" t="s">
+      <c r="H53" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="I53" s="4" t="s">
+      <c r="I53" s="1" t="s">
         <v>265</v>
       </c>
     </row>
@@ -5346,10 +5362,10 @@
       <c r="G54" t="s">
         <v>268</v>
       </c>
-      <c r="H54" s="10" t="s">
+      <c r="H54" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="I54" s="4" t="s">
+      <c r="I54" s="1" t="s">
         <v>270</v>
       </c>
     </row>
@@ -5375,10 +5391,10 @@
       <c r="G55" t="s">
         <v>273</v>
       </c>
-      <c r="H55" s="10" t="s">
+      <c r="H55" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="I55" s="4" t="s">
+      <c r="I55" s="1" t="s">
         <v>275</v>
       </c>
     </row>
@@ -5404,10 +5420,10 @@
       <c r="G56" t="s">
         <v>278</v>
       </c>
-      <c r="H56" s="10" t="s">
+      <c r="H56" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="I56" s="4" t="s">
+      <c r="I56" s="1" t="s">
         <v>280</v>
       </c>
     </row>
@@ -5433,10 +5449,10 @@
       <c r="G57" t="s">
         <v>283</v>
       </c>
-      <c r="H57" s="10" t="s">
+      <c r="H57" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="I57" s="4" t="s">
+      <c r="I57" s="1" t="s">
         <v>285</v>
       </c>
     </row>
@@ -5462,10 +5478,10 @@
       <c r="G58" t="s">
         <v>288</v>
       </c>
-      <c r="H58" s="10" t="s">
+      <c r="H58" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="I58" s="4" t="s">
+      <c r="I58" s="1" t="s">
         <v>290</v>
       </c>
     </row>
@@ -5491,10 +5507,10 @@
       <c r="G59" t="s">
         <v>293</v>
       </c>
-      <c r="H59" s="10" t="s">
+      <c r="H59" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="I59" s="4" t="s">
+      <c r="I59" s="1" t="s">
         <v>295</v>
       </c>
     </row>
@@ -5520,10 +5536,10 @@
       <c r="G60" t="s">
         <v>298</v>
       </c>
-      <c r="H60" s="10" t="s">
+      <c r="H60" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="I60" s="4" t="s">
+      <c r="I60" s="1" t="s">
         <v>300</v>
       </c>
     </row>
@@ -5549,10 +5565,10 @@
       <c r="G61" t="s">
         <v>303</v>
       </c>
-      <c r="H61" s="10" t="s">
+      <c r="H61" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="I61" s="4" t="s">
+      <c r="I61" s="1" t="s">
         <v>305</v>
       </c>
     </row>
@@ -5578,10 +5594,10 @@
       <c r="G62" t="s">
         <v>308</v>
       </c>
-      <c r="H62" s="10" t="s">
+      <c r="H62" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="I62" s="4" t="s">
+      <c r="I62" s="1" t="s">
         <v>310</v>
       </c>
     </row>
@@ -5607,10 +5623,10 @@
       <c r="G63" t="s">
         <v>313</v>
       </c>
-      <c r="H63" s="10" t="s">
+      <c r="H63" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="I63" s="4" t="s">
+      <c r="I63" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -5636,10 +5652,10 @@
       <c r="G64" t="s">
         <v>318</v>
       </c>
-      <c r="H64" s="10" t="s">
+      <c r="H64" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="I64" s="4" t="s">
+      <c r="I64" s="1" t="s">
         <v>320</v>
       </c>
     </row>
@@ -5665,10 +5681,10 @@
       <c r="G65" t="s">
         <v>323</v>
       </c>
-      <c r="H65" s="10" t="s">
+      <c r="H65" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="I65" s="4" t="s">
+      <c r="I65" s="1" t="s">
         <v>325</v>
       </c>
     </row>
@@ -5694,10 +5710,10 @@
       <c r="G66" t="s">
         <v>328</v>
       </c>
-      <c r="H66" s="10" t="s">
+      <c r="H66" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="I66" s="4" t="s">
+      <c r="I66" s="1" t="s">
         <v>330</v>
       </c>
     </row>
@@ -5723,10 +5739,10 @@
       <c r="G67" t="s">
         <v>333</v>
       </c>
-      <c r="H67" s="10" t="s">
+      <c r="H67" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="I67" s="4" t="s">
+      <c r="I67" s="1" t="s">
         <v>335</v>
       </c>
     </row>
@@ -5752,10 +5768,10 @@
       <c r="G68" t="s">
         <v>338</v>
       </c>
-      <c r="H68" s="10" t="s">
+      <c r="H68" s="5" t="s">
         <v>339</v>
       </c>
-      <c r="I68" s="4" t="s">
+      <c r="I68" s="1" t="s">
         <v>340</v>
       </c>
     </row>
@@ -5781,10 +5797,10 @@
       <c r="G69" t="s">
         <v>343</v>
       </c>
-      <c r="H69" s="10" t="s">
+      <c r="H69" s="5" t="s">
         <v>344</v>
       </c>
-      <c r="I69" s="4" t="s">
+      <c r="I69" s="1" t="s">
         <v>345</v>
       </c>
     </row>
@@ -5810,10 +5826,10 @@
       <c r="G70" t="s">
         <v>348</v>
       </c>
-      <c r="H70" s="10" t="s">
+      <c r="H70" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="I70" s="4" t="s">
+      <c r="I70" s="1" t="s">
         <v>350</v>
       </c>
     </row>
@@ -5839,10 +5855,10 @@
       <c r="G71" t="s">
         <v>353</v>
       </c>
-      <c r="H71" s="10" t="s">
+      <c r="H71" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="I71" s="4" t="s">
+      <c r="I71" s="1" t="s">
         <v>355</v>
       </c>
     </row>
@@ -5868,10 +5884,10 @@
       <c r="G72" t="s">
         <v>358</v>
       </c>
-      <c r="H72" s="10" t="s">
+      <c r="H72" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="I72" s="4" t="s">
+      <c r="I72" s="1" t="s">
         <v>360</v>
       </c>
     </row>
@@ -5897,10 +5913,10 @@
       <c r="G73" t="s">
         <v>363</v>
       </c>
-      <c r="H73" s="10" t="s">
+      <c r="H73" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="I73" s="4" t="s">
+      <c r="I73" s="1" t="s">
         <v>365</v>
       </c>
     </row>
@@ -5926,10 +5942,10 @@
       <c r="G74" t="s">
         <v>368</v>
       </c>
-      <c r="H74" s="10" t="s">
+      <c r="H74" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="I74" s="4" t="s">
+      <c r="I74" s="1" t="s">
         <v>370</v>
       </c>
     </row>
@@ -5955,10 +5971,10 @@
       <c r="G75" t="s">
         <v>988</v>
       </c>
-      <c r="H75" s="11" t="s">
+      <c r="H75" s="6" t="s">
         <v>986</v>
       </c>
-      <c r="I75" s="4" t="s">
+      <c r="I75" s="1" t="s">
         <v>990</v>
       </c>
     </row>
@@ -5984,10 +6000,10 @@
       <c r="G76" t="s">
         <v>374</v>
       </c>
-      <c r="H76" s="10" t="s">
+      <c r="H76" s="5" t="s">
         <v>375</v>
       </c>
-      <c r="I76" s="4" t="s">
+      <c r="I76" s="1" t="s">
         <v>376</v>
       </c>
     </row>
@@ -6013,10 +6029,10 @@
       <c r="G77" t="s">
         <v>379</v>
       </c>
-      <c r="H77" s="10" t="s">
+      <c r="H77" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="I77" s="4" t="s">
+      <c r="I77" s="1" t="s">
         <v>381</v>
       </c>
     </row>
@@ -6042,10 +6058,10 @@
       <c r="G78" t="s">
         <v>384</v>
       </c>
-      <c r="H78" s="10" t="s">
+      <c r="H78" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="I78" s="4" t="s">
+      <c r="I78" s="1" t="s">
         <v>386</v>
       </c>
     </row>
@@ -6071,10 +6087,10 @@
       <c r="G79" t="s">
         <v>389</v>
       </c>
-      <c r="H79" s="10" t="s">
+      <c r="H79" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="I79" s="4" t="s">
+      <c r="I79" s="1" t="s">
         <v>390</v>
       </c>
     </row>
@@ -6100,10 +6116,10 @@
       <c r="G80" t="s">
         <v>393</v>
       </c>
-      <c r="H80" s="10" t="s">
+      <c r="H80" s="5" t="s">
         <v>394</v>
       </c>
-      <c r="I80" s="4" t="s">
+      <c r="I80" s="1" t="s">
         <v>395</v>
       </c>
     </row>
@@ -6129,10 +6145,10 @@
       <c r="G81" t="s">
         <v>398</v>
       </c>
-      <c r="H81" s="10" t="s">
+      <c r="H81" s="5" t="s">
         <v>399</v>
       </c>
-      <c r="I81" s="4" t="s">
+      <c r="I81" s="1" t="s">
         <v>400</v>
       </c>
     </row>
@@ -6158,10 +6174,10 @@
       <c r="G82" t="s">
         <v>403</v>
       </c>
-      <c r="H82" s="10" t="s">
+      <c r="H82" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="I82" s="4" t="s">
+      <c r="I82" s="1" t="s">
         <v>405</v>
       </c>
     </row>
@@ -6184,10 +6200,10 @@
       <c r="G83" t="s">
         <v>408</v>
       </c>
-      <c r="H83" s="10" t="s">
+      <c r="H83" s="5" t="s">
         <v>409</v>
       </c>
-      <c r="I83" s="4" t="s">
+      <c r="I83" s="1" t="s">
         <v>410</v>
       </c>
     </row>
@@ -6213,10 +6229,10 @@
       <c r="G84" t="s">
         <v>413</v>
       </c>
-      <c r="H84" s="10" t="s">
+      <c r="H84" s="5" t="s">
         <v>414</v>
       </c>
-      <c r="I84" s="4" t="s">
+      <c r="I84" s="1" t="s">
         <v>415</v>
       </c>
     </row>
@@ -6242,10 +6258,10 @@
       <c r="G85" t="s">
         <v>418</v>
       </c>
-      <c r="H85" s="10" t="s">
+      <c r="H85" s="5" t="s">
         <v>419</v>
       </c>
-      <c r="I85" s="4" t="s">
+      <c r="I85" s="1" t="s">
         <v>420</v>
       </c>
     </row>
@@ -6271,10 +6287,10 @@
       <c r="G86" t="s">
         <v>423</v>
       </c>
-      <c r="H86" s="10" t="s">
+      <c r="H86" s="5" t="s">
         <v>424</v>
       </c>
-      <c r="I86" s="4" t="s">
+      <c r="I86" s="1" t="s">
         <v>425</v>
       </c>
     </row>
@@ -6300,10 +6316,10 @@
       <c r="G87" t="s">
         <v>428</v>
       </c>
-      <c r="H87" s="10" t="s">
+      <c r="H87" s="5" t="s">
         <v>429</v>
       </c>
-      <c r="I87" s="4" t="s">
+      <c r="I87" s="1" t="s">
         <v>430</v>
       </c>
     </row>
@@ -6329,10 +6345,10 @@
       <c r="G88" t="s">
         <v>433</v>
       </c>
-      <c r="H88" s="10" t="s">
+      <c r="H88" s="5" t="s">
         <v>434</v>
       </c>
-      <c r="I88" s="4" t="s">
+      <c r="I88" s="1" t="s">
         <v>435</v>
       </c>
     </row>
@@ -6358,10 +6374,10 @@
       <c r="G89" t="s">
         <v>438</v>
       </c>
-      <c r="H89" s="10" t="s">
+      <c r="H89" s="5" t="s">
         <v>439</v>
       </c>
-      <c r="I89" s="4" t="s">
+      <c r="I89" s="1" t="s">
         <v>440</v>
       </c>
     </row>
@@ -6387,10 +6403,10 @@
       <c r="G90" t="s">
         <v>443</v>
       </c>
-      <c r="H90" s="10" t="s">
+      <c r="H90" s="5" t="s">
         <v>444</v>
       </c>
-      <c r="I90" s="4" t="s">
+      <c r="I90" s="1" t="s">
         <v>445</v>
       </c>
     </row>
@@ -6416,10 +6432,10 @@
       <c r="G91" t="s">
         <v>448</v>
       </c>
-      <c r="H91" s="10" t="s">
+      <c r="H91" s="5" t="s">
         <v>448</v>
       </c>
-      <c r="I91" s="4" t="s">
+      <c r="I91" s="1" t="s">
         <v>449</v>
       </c>
     </row>
@@ -6445,10 +6461,10 @@
       <c r="G92" t="s">
         <v>452</v>
       </c>
-      <c r="H92" s="10" t="s">
+      <c r="H92" s="5" t="s">
         <v>453</v>
       </c>
-      <c r="I92" s="4" t="s">
+      <c r="I92" s="1" t="s">
         <v>454</v>
       </c>
     </row>
@@ -6474,10 +6490,10 @@
       <c r="G93" t="s">
         <v>457</v>
       </c>
-      <c r="H93" s="10" t="s">
+      <c r="H93" s="5" t="s">
         <v>458</v>
       </c>
-      <c r="I93" s="4" t="s">
+      <c r="I93" s="1" t="s">
         <v>459</v>
       </c>
     </row>
@@ -6503,10 +6519,10 @@
       <c r="G94" t="s">
         <v>462</v>
       </c>
-      <c r="H94" s="10" t="s">
+      <c r="H94" s="5" t="s">
         <v>463</v>
       </c>
-      <c r="I94" s="4" t="s">
+      <c r="I94" s="1" t="s">
         <v>464</v>
       </c>
     </row>
@@ -6532,10 +6548,10 @@
       <c r="G95" t="s">
         <v>467</v>
       </c>
-      <c r="H95" s="10" t="s">
+      <c r="H95" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="I95" s="4" t="s">
+      <c r="I95" s="1" t="s">
         <v>469</v>
       </c>
     </row>
@@ -6561,10 +6577,10 @@
       <c r="G96" t="s">
         <v>472</v>
       </c>
-      <c r="H96" s="10" t="s">
+      <c r="H96" s="5" t="s">
         <v>473</v>
       </c>
-      <c r="I96" s="4" t="s">
+      <c r="I96" s="1" t="s">
         <v>474</v>
       </c>
     </row>
@@ -6590,10 +6606,10 @@
       <c r="G97" t="s">
         <v>477</v>
       </c>
-      <c r="H97" s="10" t="s">
+      <c r="H97" s="5" t="s">
         <v>478</v>
       </c>
-      <c r="I97" s="4" t="s">
+      <c r="I97" s="1" t="s">
         <v>479</v>
       </c>
     </row>
@@ -6619,10 +6635,10 @@
       <c r="G98" t="s">
         <v>482</v>
       </c>
-      <c r="H98" s="10" t="s">
+      <c r="H98" s="5" t="s">
         <v>483</v>
       </c>
-      <c r="I98" s="4" t="s">
+      <c r="I98" s="1" t="s">
         <v>484</v>
       </c>
     </row>
@@ -6648,10 +6664,10 @@
       <c r="G99" t="s">
         <v>487</v>
       </c>
-      <c r="H99" s="10" t="s">
+      <c r="H99" s="5" t="s">
         <v>488</v>
       </c>
-      <c r="I99" s="4" t="s">
+      <c r="I99" s="1" t="s">
         <v>489</v>
       </c>
     </row>
@@ -6677,10 +6693,10 @@
       <c r="G100" t="s">
         <v>492</v>
       </c>
-      <c r="H100" s="10" t="s">
+      <c r="H100" s="5" t="s">
         <v>493</v>
       </c>
-      <c r="I100" s="4" t="s">
+      <c r="I100" s="1" t="s">
         <v>494</v>
       </c>
     </row>
@@ -6703,10 +6719,10 @@
       <c r="G101" t="s">
         <v>497</v>
       </c>
-      <c r="H101" s="10" t="s">
+      <c r="H101" s="5" t="s">
         <v>497</v>
       </c>
-      <c r="I101" s="4" t="s">
+      <c r="I101" s="1" t="s">
         <v>498</v>
       </c>
     </row>
@@ -6732,10 +6748,10 @@
       <c r="G102" t="s">
         <v>501</v>
       </c>
-      <c r="H102" s="10" t="s">
+      <c r="H102" s="5" t="s">
         <v>502</v>
       </c>
-      <c r="I102" s="4" t="s">
+      <c r="I102" s="1" t="s">
         <v>503</v>
       </c>
     </row>
@@ -6761,10 +6777,10 @@
       <c r="G103" t="s">
         <v>506</v>
       </c>
-      <c r="H103" s="10" t="s">
+      <c r="H103" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="I103" s="4" t="s">
+      <c r="I103" s="1" t="s">
         <v>508</v>
       </c>
     </row>
@@ -6790,10 +6806,10 @@
       <c r="G104" t="s">
         <v>511</v>
       </c>
-      <c r="H104" s="10" t="s">
+      <c r="H104" s="5" t="s">
         <v>512</v>
       </c>
-      <c r="I104" s="4" t="s">
+      <c r="I104" s="1" t="s">
         <v>513</v>
       </c>
     </row>
@@ -6819,10 +6835,10 @@
       <c r="G105" t="s">
         <v>516</v>
       </c>
-      <c r="H105" s="10" t="s">
+      <c r="H105" s="5" t="s">
         <v>517</v>
       </c>
-      <c r="I105" s="4" t="s">
+      <c r="I105" s="1" t="s">
         <v>518</v>
       </c>
     </row>
@@ -6848,10 +6864,10 @@
       <c r="G106" t="s">
         <v>521</v>
       </c>
-      <c r="H106" s="10" t="s">
+      <c r="H106" s="5" t="s">
         <v>522</v>
       </c>
-      <c r="I106" s="4" t="s">
+      <c r="I106" s="1" t="s">
         <v>523</v>
       </c>
     </row>
@@ -6877,10 +6893,10 @@
       <c r="G107" t="s">
         <v>526</v>
       </c>
-      <c r="H107" s="10" t="s">
+      <c r="H107" s="5" t="s">
         <v>527</v>
       </c>
-      <c r="I107" s="4" t="s">
+      <c r="I107" s="1" t="s">
         <v>528</v>
       </c>
     </row>
@@ -6906,10 +6922,10 @@
       <c r="G108" t="s">
         <v>531</v>
       </c>
-      <c r="H108" s="10" t="s">
+      <c r="H108" s="5" t="s">
         <v>532</v>
       </c>
-      <c r="I108" s="4" t="s">
+      <c r="I108" s="1" t="s">
         <v>533</v>
       </c>
     </row>
@@ -6935,10 +6951,10 @@
       <c r="G109" t="s">
         <v>536</v>
       </c>
-      <c r="H109" s="10" t="s">
+      <c r="H109" s="5" t="s">
         <v>537</v>
       </c>
-      <c r="I109" s="4" t="s">
+      <c r="I109" s="1" t="s">
         <v>538</v>
       </c>
     </row>
@@ -6964,10 +6980,10 @@
       <c r="G110" t="s">
         <v>541</v>
       </c>
-      <c r="H110" s="10" t="s">
+      <c r="H110" s="5" t="s">
         <v>542</v>
       </c>
-      <c r="I110" s="4" t="s">
+      <c r="I110" s="1" t="s">
         <v>543</v>
       </c>
     </row>
@@ -6993,10 +7009,10 @@
       <c r="G111" t="s">
         <v>546</v>
       </c>
-      <c r="H111" s="10" t="s">
+      <c r="H111" s="5" t="s">
         <v>547</v>
       </c>
-      <c r="I111" s="4" t="s">
+      <c r="I111" s="1" t="s">
         <v>548</v>
       </c>
     </row>
@@ -7022,10 +7038,10 @@
       <c r="G112" t="s">
         <v>551</v>
       </c>
-      <c r="H112" s="10" t="s">
+      <c r="H112" s="5" t="s">
         <v>552</v>
       </c>
-      <c r="I112" s="4" t="s">
+      <c r="I112" s="1" t="s">
         <v>553</v>
       </c>
     </row>
@@ -7051,10 +7067,10 @@
       <c r="G113" t="s">
         <v>556</v>
       </c>
-      <c r="H113" s="10" t="s">
+      <c r="H113" s="5" t="s">
         <v>557</v>
       </c>
-      <c r="I113" s="4" t="s">
+      <c r="I113" s="1" t="s">
         <v>558</v>
       </c>
     </row>
@@ -7080,10 +7096,10 @@
       <c r="G114" t="s">
         <v>561</v>
       </c>
-      <c r="H114" s="10" t="s">
+      <c r="H114" s="5" t="s">
         <v>562</v>
       </c>
-      <c r="I114" s="4" t="s">
+      <c r="I114" s="1" t="s">
         <v>563</v>
       </c>
     </row>
@@ -7109,10 +7125,10 @@
       <c r="G115" t="s">
         <v>566</v>
       </c>
-      <c r="H115" s="10" t="s">
+      <c r="H115" s="5" t="s">
         <v>567</v>
       </c>
-      <c r="I115" s="4" t="s">
+      <c r="I115" s="1" t="s">
         <v>568</v>
       </c>
     </row>
@@ -7138,10 +7154,10 @@
       <c r="G116" t="s">
         <v>571</v>
       </c>
-      <c r="H116" s="10" t="s">
+      <c r="H116" s="5" t="s">
         <v>571</v>
       </c>
-      <c r="I116" s="4" t="s">
+      <c r="I116" s="1" t="s">
         <v>572</v>
       </c>
     </row>
@@ -7167,10 +7183,10 @@
       <c r="G117" t="s">
         <v>575</v>
       </c>
-      <c r="H117" s="10" t="s">
+      <c r="H117" s="5" t="s">
         <v>576</v>
       </c>
-      <c r="I117" s="4" t="s">
+      <c r="I117" s="1" t="s">
         <v>577</v>
       </c>
     </row>
@@ -7196,10 +7212,10 @@
       <c r="G118" t="s">
         <v>580</v>
       </c>
-      <c r="H118" s="10" t="s">
+      <c r="H118" s="5" t="s">
         <v>581</v>
       </c>
-      <c r="I118" s="4" t="s">
+      <c r="I118" s="1" t="s">
         <v>582</v>
       </c>
     </row>
@@ -7225,10 +7241,10 @@
       <c r="G119" t="s">
         <v>585</v>
       </c>
-      <c r="H119" s="10" t="s">
+      <c r="H119" s="5" t="s">
         <v>586</v>
       </c>
-      <c r="I119" s="4" t="s">
+      <c r="I119" s="1" t="s">
         <v>587</v>
       </c>
     </row>
@@ -7254,10 +7270,10 @@
       <c r="G120" t="s">
         <v>590</v>
       </c>
-      <c r="H120" s="10" t="s">
+      <c r="H120" s="5" t="s">
         <v>591</v>
       </c>
-      <c r="I120" s="4" t="s">
+      <c r="I120" s="1" t="s">
         <v>592</v>
       </c>
     </row>
@@ -7283,10 +7299,10 @@
       <c r="G121" t="s">
         <v>595</v>
       </c>
-      <c r="H121" s="10" t="s">
+      <c r="H121" s="5" t="s">
         <v>596</v>
       </c>
-      <c r="I121" s="4" t="s">
+      <c r="I121" s="1" t="s">
         <v>597</v>
       </c>
     </row>
@@ -7309,10 +7325,10 @@
       <c r="G122" t="s">
         <v>1076</v>
       </c>
-      <c r="H122" s="10" t="s">
+      <c r="H122" s="5" t="s">
         <v>1077</v>
       </c>
-      <c r="I122" s="4" t="s">
+      <c r="I122" s="1" t="s">
         <v>1078</v>
       </c>
     </row>
@@ -7338,10 +7354,10 @@
       <c r="G123" t="s">
         <v>601</v>
       </c>
-      <c r="H123" s="10" t="s">
+      <c r="H123" s="5" t="s">
         <v>602</v>
       </c>
-      <c r="I123" s="4" t="s">
+      <c r="I123" s="1" t="s">
         <v>603</v>
       </c>
     </row>
@@ -7367,10 +7383,10 @@
       <c r="G124" t="s">
         <v>606</v>
       </c>
-      <c r="H124" s="10" t="s">
+      <c r="H124" s="5" t="s">
         <v>607</v>
       </c>
-      <c r="I124" s="4" t="s">
+      <c r="I124" s="1" t="s">
         <v>608</v>
       </c>
     </row>
@@ -7396,10 +7412,10 @@
       <c r="G125" t="s">
         <v>611</v>
       </c>
-      <c r="H125" s="10" t="s">
+      <c r="H125" s="5" t="s">
         <v>612</v>
       </c>
-      <c r="I125" s="4" t="s">
+      <c r="I125" s="1" t="s">
         <v>613</v>
       </c>
     </row>
@@ -7425,10 +7441,10 @@
       <c r="G126" t="s">
         <v>616</v>
       </c>
-      <c r="H126" s="10" t="s">
+      <c r="H126" s="5" t="s">
         <v>617</v>
       </c>
-      <c r="I126" s="4" t="s">
+      <c r="I126" s="1" t="s">
         <v>618</v>
       </c>
     </row>
@@ -7454,10 +7470,10 @@
       <c r="G127" t="s">
         <v>621</v>
       </c>
-      <c r="H127" s="10" t="s">
+      <c r="H127" s="5" t="s">
         <v>622</v>
       </c>
-      <c r="I127" s="4" t="s">
+      <c r="I127" s="1" t="s">
         <v>623</v>
       </c>
     </row>
@@ -7483,10 +7499,10 @@
       <c r="G128" t="s">
         <v>1071</v>
       </c>
-      <c r="H128" s="10" t="s">
+      <c r="H128" s="5" t="s">
         <v>626</v>
       </c>
-      <c r="I128" s="4" t="s">
+      <c r="I128" s="1" t="s">
         <v>627</v>
       </c>
     </row>
@@ -7512,10 +7528,10 @@
       <c r="G129" t="s">
         <v>630</v>
       </c>
-      <c r="H129" s="10" t="s">
+      <c r="H129" s="5" t="s">
         <v>631</v>
       </c>
-      <c r="I129" s="4" t="s">
+      <c r="I129" s="1" t="s">
         <v>632</v>
       </c>
     </row>
@@ -7541,10 +7557,10 @@
       <c r="G130" t="s">
         <v>635</v>
       </c>
-      <c r="H130" s="10" t="s">
+      <c r="H130" s="5" t="s">
         <v>636</v>
       </c>
-      <c r="I130" s="4" t="s">
+      <c r="I130" s="1" t="s">
         <v>637</v>
       </c>
     </row>
@@ -7570,10 +7586,10 @@
       <c r="G131" t="s">
         <v>640</v>
       </c>
-      <c r="H131" s="10" t="s">
+      <c r="H131" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="I131" s="4" t="s">
+      <c r="I131" s="1" t="s">
         <v>642</v>
       </c>
     </row>
@@ -7599,10 +7615,10 @@
       <c r="G132" t="s">
         <v>645</v>
       </c>
-      <c r="H132" s="10" t="s">
+      <c r="H132" s="5" t="s">
         <v>646</v>
       </c>
-      <c r="I132" s="4" t="s">
+      <c r="I132" s="1" t="s">
         <v>647</v>
       </c>
     </row>
@@ -7628,10 +7644,10 @@
       <c r="G133" t="s">
         <v>650</v>
       </c>
-      <c r="H133" s="10" t="s">
+      <c r="H133" s="5" t="s">
         <v>651</v>
       </c>
-      <c r="I133" s="4" t="s">
+      <c r="I133" s="1" t="s">
         <v>652</v>
       </c>
     </row>
@@ -7657,10 +7673,10 @@
       <c r="G134" t="s">
         <v>655</v>
       </c>
-      <c r="H134" s="10" t="s">
+      <c r="H134" s="5" t="s">
         <v>656</v>
       </c>
-      <c r="I134" s="4" t="s">
+      <c r="I134" s="1" t="s">
         <v>657</v>
       </c>
     </row>
@@ -7686,10 +7702,10 @@
       <c r="G135" t="s">
         <v>660</v>
       </c>
-      <c r="H135" s="10" t="s">
+      <c r="H135" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="I135" s="4" t="s">
+      <c r="I135" s="1" t="s">
         <v>662</v>
       </c>
     </row>
@@ -7715,10 +7731,10 @@
       <c r="G136" t="s">
         <v>665</v>
       </c>
-      <c r="H136" s="10" t="s">
+      <c r="H136" s="5" t="s">
         <v>666</v>
       </c>
-      <c r="I136" s="4" t="s">
+      <c r="I136" s="1" t="s">
         <v>667</v>
       </c>
     </row>
@@ -7744,10 +7760,10 @@
       <c r="G137" t="s">
         <v>670</v>
       </c>
-      <c r="H137" s="10" t="s">
+      <c r="H137" s="5" t="s">
         <v>671</v>
       </c>
-      <c r="I137" s="4" t="s">
+      <c r="I137" s="1" t="s">
         <v>672</v>
       </c>
     </row>
@@ -7773,10 +7789,10 @@
       <c r="G138" t="s">
         <v>675</v>
       </c>
-      <c r="H138" s="10" t="s">
+      <c r="H138" s="5" t="s">
         <v>676</v>
       </c>
-      <c r="I138" s="4" t="s">
+      <c r="I138" s="1" t="s">
         <v>677</v>
       </c>
     </row>
@@ -7802,10 +7818,10 @@
       <c r="G139" t="s">
         <v>680</v>
       </c>
-      <c r="H139" s="10" t="s">
+      <c r="H139" s="5" t="s">
         <v>680</v>
       </c>
-      <c r="I139" s="4" t="s">
+      <c r="I139" s="1" t="s">
         <v>681</v>
       </c>
     </row>
@@ -7831,10 +7847,10 @@
       <c r="G140" t="s">
         <v>684</v>
       </c>
-      <c r="H140" s="10" t="s">
+      <c r="H140" s="5" t="s">
         <v>685</v>
       </c>
-      <c r="I140" s="4" t="s">
+      <c r="I140" s="1" t="s">
         <v>686</v>
       </c>
     </row>
@@ -7860,10 +7876,10 @@
       <c r="G141" t="s">
         <v>689</v>
       </c>
-      <c r="H141" s="10" t="s">
+      <c r="H141" s="5" t="s">
         <v>690</v>
       </c>
-      <c r="I141" s="4" t="s">
+      <c r="I141" s="1" t="s">
         <v>691</v>
       </c>
     </row>
@@ -7889,10 +7905,10 @@
       <c r="G142" t="s">
         <v>694</v>
       </c>
-      <c r="H142" s="10" t="s">
+      <c r="H142" s="5" t="s">
         <v>695</v>
       </c>
-      <c r="I142" s="4" t="s">
+      <c r="I142" s="1" t="s">
         <v>696</v>
       </c>
     </row>
@@ -7918,10 +7934,10 @@
       <c r="G143" t="s">
         <v>699</v>
       </c>
-      <c r="H143" s="10" t="s">
+      <c r="H143" s="5" t="s">
         <v>700</v>
       </c>
-      <c r="I143" s="4" t="s">
+      <c r="I143" s="1" t="s">
         <v>701</v>
       </c>
     </row>
@@ -7947,10 +7963,10 @@
       <c r="G144" t="s">
         <v>704</v>
       </c>
-      <c r="H144" s="10" t="s">
+      <c r="H144" s="5" t="s">
         <v>705</v>
       </c>
-      <c r="I144" s="4" t="s">
+      <c r="I144" s="1" t="s">
         <v>706</v>
       </c>
     </row>
@@ -7976,10 +7992,10 @@
       <c r="G145" t="s">
         <v>709</v>
       </c>
-      <c r="H145" s="10" t="s">
+      <c r="H145" s="5" t="s">
         <v>710</v>
       </c>
-      <c r="I145" s="4" t="s">
+      <c r="I145" s="1" t="s">
         <v>711</v>
       </c>
     </row>
@@ -8005,10 +8021,10 @@
       <c r="G146" t="s">
         <v>714</v>
       </c>
-      <c r="H146" s="10" t="s">
+      <c r="H146" s="5" t="s">
         <v>715</v>
       </c>
-      <c r="I146" s="4" t="s">
+      <c r="I146" s="1" t="s">
         <v>716</v>
       </c>
     </row>
@@ -8034,10 +8050,10 @@
       <c r="G147" t="s">
         <v>719</v>
       </c>
-      <c r="H147" s="10" t="s">
+      <c r="H147" s="5" t="s">
         <v>720</v>
       </c>
-      <c r="I147" s="4" t="s">
+      <c r="I147" s="1" t="s">
         <v>721</v>
       </c>
     </row>
@@ -8063,10 +8079,10 @@
       <c r="G148" t="s">
         <v>724</v>
       </c>
-      <c r="H148" s="10" t="s">
+      <c r="H148" s="5" t="s">
         <v>725</v>
       </c>
-      <c r="I148" s="4" t="s">
+      <c r="I148" s="1" t="s">
         <v>726</v>
       </c>
     </row>
@@ -8092,10 +8108,10 @@
       <c r="G149" t="s">
         <v>729</v>
       </c>
-      <c r="H149" s="10" t="s">
+      <c r="H149" s="5" t="s">
         <v>730</v>
       </c>
-      <c r="I149" s="4" t="s">
+      <c r="I149" s="1" t="s">
         <v>731</v>
       </c>
     </row>
@@ -8121,10 +8137,10 @@
       <c r="G150" t="s">
         <v>734</v>
       </c>
-      <c r="H150" s="10" t="s">
+      <c r="H150" s="5" t="s">
         <v>735</v>
       </c>
-      <c r="I150" s="4" t="s">
+      <c r="I150" s="1" t="s">
         <v>736</v>
       </c>
     </row>
@@ -8150,10 +8166,10 @@
       <c r="G151" t="s">
         <v>739</v>
       </c>
-      <c r="H151" s="10" t="s">
+      <c r="H151" s="5" t="s">
         <v>740</v>
       </c>
-      <c r="I151" s="4" t="s">
+      <c r="I151" s="1" t="s">
         <v>741</v>
       </c>
     </row>
@@ -8179,10 +8195,10 @@
       <c r="G152" t="s">
         <v>744</v>
       </c>
-      <c r="H152" s="10" t="s">
+      <c r="H152" s="5" t="s">
         <v>745</v>
       </c>
-      <c r="I152" s="4" t="s">
+      <c r="I152" s="1" t="s">
         <v>746</v>
       </c>
     </row>
@@ -8208,10 +8224,10 @@
       <c r="G153" t="s">
         <v>939</v>
       </c>
-      <c r="H153" s="12" t="s">
+      <c r="H153" s="7" t="s">
         <v>1017</v>
       </c>
-      <c r="I153" s="5" t="s">
+      <c r="I153" s="2" t="s">
         <v>1018</v>
       </c>
     </row>
@@ -8237,7 +8253,7 @@
       <c r="G154" t="s">
         <v>942</v>
       </c>
-      <c r="H154" s="11" t="s">
+      <c r="H154" s="6" t="s">
         <v>978</v>
       </c>
     </row>
@@ -8263,7 +8279,7 @@
       <c r="G155" t="s">
         <v>945</v>
       </c>
-      <c r="H155" s="11" t="s">
+      <c r="H155" s="6" t="s">
         <v>1063</v>
       </c>
     </row>
@@ -8289,7 +8305,7 @@
       <c r="G156" t="s">
         <v>948</v>
       </c>
-      <c r="H156" s="11" t="s">
+      <c r="H156" s="6" t="s">
         <v>1045</v>
       </c>
     </row>
@@ -8315,7 +8331,7 @@
       <c r="G157" t="s">
         <v>951</v>
       </c>
-      <c r="H157" s="13" t="s">
+      <c r="H157" s="8" t="s">
         <v>1032</v>
       </c>
     </row>
@@ -8341,7 +8357,7 @@
       <c r="G158" t="s">
         <v>954</v>
       </c>
-      <c r="H158" s="11" t="s">
+      <c r="H158" s="6" t="s">
         <v>1048</v>
       </c>
     </row>
@@ -8367,7 +8383,7 @@
       <c r="G159" t="s">
         <v>957</v>
       </c>
-      <c r="H159" s="11" t="s">
+      <c r="H159" s="6" t="s">
         <v>1050</v>
       </c>
     </row>
@@ -8393,7 +8409,7 @@
       <c r="G160" t="s">
         <v>960</v>
       </c>
-      <c r="H160" s="13" t="s">
+      <c r="H160" s="8" t="s">
         <v>1051</v>
       </c>
     </row>
@@ -8419,7 +8435,7 @@
       <c r="G161" t="s">
         <v>963</v>
       </c>
-      <c r="H161" s="11" t="s">
+      <c r="H161" s="6" t="s">
         <v>1054</v>
       </c>
     </row>
@@ -8445,10 +8461,10 @@
       <c r="G162" t="s">
         <v>482</v>
       </c>
-      <c r="H162" s="10" t="s">
+      <c r="H162" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="I162" s="4" t="s">
+      <c r="I162" s="1" t="s">
         <v>1065</v>
       </c>
     </row>
@@ -8474,7 +8490,7 @@
       <c r="G163" t="s">
         <v>814</v>
       </c>
-      <c r="H163" s="11" t="s">
+      <c r="H163" s="6" t="s">
         <v>974</v>
       </c>
     </row>
@@ -8500,7 +8516,7 @@
       <c r="G164" t="s">
         <v>817</v>
       </c>
-      <c r="H164" s="11" t="s">
+      <c r="H164" s="6" t="s">
         <v>1023</v>
       </c>
     </row>
@@ -8526,7 +8542,7 @@
       <c r="G165" t="s">
         <v>820</v>
       </c>
-      <c r="H165" s="11" t="s">
+      <c r="H165" s="6" t="s">
         <v>1022</v>
       </c>
     </row>
@@ -8552,7 +8568,7 @@
       <c r="G166" t="s">
         <v>823</v>
       </c>
-      <c r="H166" s="11" t="s">
+      <c r="H166" s="6" t="s">
         <v>1033</v>
       </c>
     </row>
@@ -8578,7 +8594,7 @@
       <c r="G167" t="s">
         <v>826</v>
       </c>
-      <c r="H167" s="11" t="s">
+      <c r="H167" s="6" t="s">
         <v>1049</v>
       </c>
     </row>
@@ -8604,7 +8620,7 @@
       <c r="G168" t="s">
         <v>829</v>
       </c>
-      <c r="H168" s="11" t="s">
+      <c r="H168" s="6" t="s">
         <v>1052</v>
       </c>
     </row>
@@ -8630,7 +8646,7 @@
       <c r="G169" t="s">
         <v>832</v>
       </c>
-      <c r="H169" s="11" t="s">
+      <c r="H169" s="6" t="s">
         <v>1056</v>
       </c>
     </row>
@@ -8656,7 +8672,7 @@
       <c r="G170" t="s">
         <v>835</v>
       </c>
-      <c r="H170" s="13" t="s">
+      <c r="H170" s="8" t="s">
         <v>1057</v>
       </c>
     </row>
@@ -8682,7 +8698,7 @@
       <c r="G171" t="s">
         <v>865</v>
       </c>
-      <c r="H171" s="11" t="s">
+      <c r="H171" s="6" t="s">
         <v>967</v>
       </c>
     </row>
@@ -8708,7 +8724,7 @@
       <c r="G172" t="s">
         <v>868</v>
       </c>
-      <c r="H172" s="11" t="s">
+      <c r="H172" s="6" t="s">
         <v>968</v>
       </c>
     </row>
@@ -8734,7 +8750,7 @@
       <c r="G173" t="s">
         <v>886</v>
       </c>
-      <c r="H173" s="12" t="s">
+      <c r="H173" s="7" t="s">
         <v>1064</v>
       </c>
     </row>
@@ -8760,7 +8776,7 @@
       <c r="G174" t="s">
         <v>889</v>
       </c>
-      <c r="H174" s="11" t="s">
+      <c r="H174" s="6" t="s">
         <v>973</v>
       </c>
     </row>
@@ -8786,7 +8802,7 @@
       <c r="G175" t="s">
         <v>892</v>
       </c>
-      <c r="H175" s="11" t="s">
+      <c r="H175" s="6" t="s">
         <v>977</v>
       </c>
     </row>
@@ -8812,7 +8828,7 @@
       <c r="G176" t="s">
         <v>895</v>
       </c>
-      <c r="H176" s="11" t="s">
+      <c r="H176" s="6" t="s">
         <v>979</v>
       </c>
     </row>
@@ -8838,7 +8854,7 @@
       <c r="G177" t="s">
         <v>898</v>
       </c>
-      <c r="H177" s="11" t="s">
+      <c r="H177" s="6" t="s">
         <v>980</v>
       </c>
     </row>
@@ -8864,7 +8880,7 @@
       <c r="G178" t="s">
         <v>901</v>
       </c>
-      <c r="H178" s="11" t="s">
+      <c r="H178" s="6" t="s">
         <v>981</v>
       </c>
     </row>
@@ -8890,7 +8906,7 @@
       <c r="G179" t="s">
         <v>904</v>
       </c>
-      <c r="H179" s="11" t="s">
+      <c r="H179" s="6" t="s">
         <v>1023</v>
       </c>
     </row>
@@ -8916,7 +8932,7 @@
       <c r="G180" t="s">
         <v>907</v>
       </c>
-      <c r="H180" s="13" t="s">
+      <c r="H180" s="8" t="s">
         <v>1044</v>
       </c>
     </row>
@@ -8942,7 +8958,7 @@
       <c r="G181" t="s">
         <v>910</v>
       </c>
-      <c r="H181" s="11" t="s">
+      <c r="H181" s="6" t="s">
         <v>1067</v>
       </c>
     </row>
@@ -8968,7 +8984,7 @@
       <c r="G182" t="s">
         <v>913</v>
       </c>
-      <c r="H182" s="13" t="s">
+      <c r="H182" s="8" t="s">
         <v>1055</v>
       </c>
     </row>
@@ -8994,10 +9010,10 @@
       <c r="G183" t="s">
         <v>883</v>
       </c>
-      <c r="H183" s="14" t="s">
+      <c r="H183" s="9" t="s">
         <v>1019</v>
       </c>
-      <c r="I183" s="6" t="s">
+      <c r="I183" s="3" t="s">
         <v>1020</v>
       </c>
     </row>
@@ -9023,7 +9039,7 @@
       <c r="G184" t="s">
         <v>783</v>
       </c>
-      <c r="H184" s="11" t="s">
+      <c r="H184" s="6" t="s">
         <v>966</v>
       </c>
     </row>
@@ -9049,7 +9065,7 @@
       <c r="G185" t="s">
         <v>997</v>
       </c>
-      <c r="H185" s="11" t="s">
+      <c r="H185" s="6" t="s">
         <v>1058</v>
       </c>
     </row>
@@ -9075,7 +9091,7 @@
       <c r="G186" t="s">
         <v>1000</v>
       </c>
-      <c r="H186" s="11" t="s">
+      <c r="H186" s="6" t="s">
         <v>1059</v>
       </c>
     </row>
@@ -9101,7 +9117,7 @@
       <c r="G187" t="s">
         <v>936</v>
       </c>
-      <c r="H187" s="11" t="s">
+      <c r="H187" s="6" t="s">
         <v>984</v>
       </c>
     </row>
@@ -9127,7 +9143,7 @@
       <c r="G188" t="s">
         <v>796</v>
       </c>
-      <c r="H188" s="13" t="s">
+      <c r="H188" s="8" t="s">
         <v>1060</v>
       </c>
     </row>
@@ -9153,7 +9169,7 @@
       <c r="G189" t="s">
         <v>799</v>
       </c>
-      <c r="H189" s="13" t="s">
+      <c r="H189" s="8" t="s">
         <v>1061</v>
       </c>
     </row>
@@ -9179,7 +9195,7 @@
       <c r="G190" t="s">
         <v>802</v>
       </c>
-      <c r="H190" s="11" t="s">
+      <c r="H190" s="6" t="s">
         <v>985</v>
       </c>
     </row>
@@ -9205,7 +9221,7 @@
       <c r="G191" t="s">
         <v>805</v>
       </c>
-      <c r="H191" s="11" t="s">
+      <c r="H191" s="6" t="s">
         <v>1035</v>
       </c>
     </row>
@@ -9231,7 +9247,7 @@
       <c r="G192" t="s">
         <v>808</v>
       </c>
-      <c r="H192" s="11" t="s">
+      <c r="H192" s="6" t="s">
         <v>1041</v>
       </c>
     </row>
@@ -9257,7 +9273,7 @@
       <c r="G193" t="s">
         <v>811</v>
       </c>
-      <c r="H193" s="11" t="s">
+      <c r="H193" s="6" t="s">
         <v>1034</v>
       </c>
     </row>
@@ -9283,7 +9299,7 @@
       <c r="G194" t="s">
         <v>994</v>
       </c>
-      <c r="H194" s="11" t="s">
+      <c r="H194" s="6" t="s">
         <v>1042</v>
       </c>
     </row>
@@ -9309,7 +9325,7 @@
       <c r="G195" t="s">
         <v>759</v>
       </c>
-      <c r="H195" s="13" t="s">
+      <c r="H195" s="8" t="s">
         <v>964</v>
       </c>
     </row>
@@ -9335,7 +9351,7 @@
       <c r="G196" t="s">
         <v>762</v>
       </c>
-      <c r="H196" s="11" t="s">
+      <c r="H196" s="6" t="s">
         <v>969</v>
       </c>
     </row>
@@ -9361,7 +9377,7 @@
       <c r="G197" t="s">
         <v>765</v>
       </c>
-      <c r="H197" s="11" t="s">
+      <c r="H197" s="6" t="s">
         <v>1046</v>
       </c>
     </row>
@@ -9387,7 +9403,7 @@
       <c r="G198" t="s">
         <v>768</v>
       </c>
-      <c r="H198" s="11" t="s">
+      <c r="H198" s="6" t="s">
         <v>1025</v>
       </c>
     </row>
@@ -9413,7 +9429,7 @@
       <c r="G199" t="s">
         <v>771</v>
       </c>
-      <c r="H199" s="11" t="s">
+      <c r="H199" s="6" t="s">
         <v>1030</v>
       </c>
     </row>
@@ -9439,7 +9455,7 @@
       <c r="G200" t="s">
         <v>774</v>
       </c>
-      <c r="H200" s="11" t="s">
+      <c r="H200" s="6" t="s">
         <v>1028</v>
       </c>
     </row>
@@ -9465,7 +9481,7 @@
       <c r="G201" t="s">
         <v>777</v>
       </c>
-      <c r="H201" s="11" t="s">
+      <c r="H201" s="6" t="s">
         <v>1038</v>
       </c>
     </row>
@@ -9491,7 +9507,7 @@
       <c r="G202" t="s">
         <v>780</v>
       </c>
-      <c r="H202" s="11" t="s">
+      <c r="H202" s="6" t="s">
         <v>1053</v>
       </c>
     </row>
@@ -9517,7 +9533,7 @@
       <c r="G203" t="s">
         <v>838</v>
       </c>
-      <c r="H203" s="11" t="s">
+      <c r="H203" s="6" t="s">
         <v>965</v>
       </c>
     </row>
@@ -9543,7 +9559,7 @@
       <c r="G204" t="s">
         <v>841</v>
       </c>
-      <c r="H204" s="11" t="s">
+      <c r="H204" s="6" t="s">
         <v>975</v>
       </c>
     </row>
@@ -9569,7 +9585,7 @@
       <c r="G205" t="s">
         <v>844</v>
       </c>
-      <c r="H205" s="11" t="s">
+      <c r="H205" s="6" t="s">
         <v>976</v>
       </c>
     </row>
@@ -9595,7 +9611,7 @@
       <c r="G206" t="s">
         <v>847</v>
       </c>
-      <c r="H206" s="13" t="s">
+      <c r="H206" s="8" t="s">
         <v>1027</v>
       </c>
     </row>
@@ -9621,7 +9637,7 @@
       <c r="G207" t="s">
         <v>850</v>
       </c>
-      <c r="H207" s="13" t="s">
+      <c r="H207" s="8" t="s">
         <v>1026</v>
       </c>
     </row>
@@ -9647,7 +9663,7 @@
       <c r="G208" t="s">
         <v>853</v>
       </c>
-      <c r="H208" s="11" t="s">
+      <c r="H208" s="6" t="s">
         <v>1040</v>
       </c>
     </row>
@@ -9673,7 +9689,7 @@
       <c r="G209" t="s">
         <v>856</v>
       </c>
-      <c r="H209" s="11" t="s">
+      <c r="H209" s="6" t="s">
         <v>1037</v>
       </c>
     </row>
@@ -9699,7 +9715,7 @@
       <c r="G210" t="s">
         <v>859</v>
       </c>
-      <c r="H210" s="11" t="s">
+      <c r="H210" s="6" t="s">
         <v>1043</v>
       </c>
     </row>
@@ -9725,7 +9741,7 @@
       <c r="G211" t="s">
         <v>862</v>
       </c>
-      <c r="H211" s="11" t="s">
+      <c r="H211" s="6" t="s">
         <v>1047</v>
       </c>
     </row>
@@ -9751,7 +9767,7 @@
       <c r="G212" t="s">
         <v>916</v>
       </c>
-      <c r="H212" s="13" t="s">
+      <c r="H212" s="8" t="s">
         <v>1024</v>
       </c>
     </row>
@@ -9777,7 +9793,7 @@
       <c r="G213" t="s">
         <v>919</v>
       </c>
-      <c r="H213" s="11" t="s">
+      <c r="H213" s="6" t="s">
         <v>1029</v>
       </c>
     </row>
@@ -9803,7 +9819,7 @@
       <c r="G214" t="s">
         <v>922</v>
       </c>
-      <c r="H214" s="11" t="s">
+      <c r="H214" s="6" t="s">
         <v>1031</v>
       </c>
     </row>
@@ -9829,7 +9845,7 @@
       <c r="G215" t="s">
         <v>925</v>
       </c>
-      <c r="H215" s="13" t="s">
+      <c r="H215" s="8" t="s">
         <v>1036</v>
       </c>
     </row>
@@ -9855,7 +9871,7 @@
       <c r="G216" t="s">
         <v>928</v>
       </c>
-      <c r="H216" s="11" t="s">
+      <c r="H216" s="6" t="s">
         <v>1043</v>
       </c>
     </row>
@@ -9881,7 +9897,7 @@
       <c r="G217" t="s">
         <v>931</v>
       </c>
-      <c r="H217" s="11" t="s">
+      <c r="H217" s="6" t="s">
         <v>1062</v>
       </c>
     </row>
@@ -9907,7 +9923,7 @@
       <c r="G218" t="s">
         <v>1007</v>
       </c>
-      <c r="H218" s="11" t="s">
+      <c r="H218" s="6" t="s">
         <v>1039</v>
       </c>
     </row>
@@ -9933,7 +9949,7 @@
       <c r="G219" t="s">
         <v>933</v>
       </c>
-      <c r="H219" s="11" t="s">
+      <c r="H219" s="6" t="s">
         <v>983</v>
       </c>
     </row>
@@ -9959,7 +9975,7 @@
       <c r="G220" t="s">
         <v>786</v>
       </c>
-      <c r="H220" s="13" t="s">
+      <c r="H220" s="8" t="s">
         <v>972</v>
       </c>
     </row>
@@ -9985,7 +10001,7 @@
       <c r="G221" t="s">
         <v>789</v>
       </c>
-      <c r="H221" s="11" t="s">
+      <c r="H221" s="6" t="s">
         <v>1021</v>
       </c>
     </row>
@@ -10011,7 +10027,7 @@
       <c r="G222" t="s">
         <v>792</v>
       </c>
-      <c r="H222" s="11" t="s">
+      <c r="H222" s="6" t="s">
         <v>982</v>
       </c>
     </row>
@@ -10037,7 +10053,7 @@
       <c r="G223" t="s">
         <v>871</v>
       </c>
-      <c r="H223" s="11" t="s">
+      <c r="H223" s="6" t="s">
         <v>970</v>
       </c>
     </row>
@@ -10063,7 +10079,7 @@
       <c r="G224" t="s">
         <v>874</v>
       </c>
-      <c r="H224" s="11" t="s">
+      <c r="H224" s="6" t="s">
         <v>971</v>
       </c>
     </row>
@@ -10089,7 +10105,7 @@
       <c r="G225" t="s">
         <v>877</v>
       </c>
-      <c r="H225" s="11" t="s">
+      <c r="H225" s="6" t="s">
         <v>1021</v>
       </c>
     </row>
@@ -10115,10 +10131,10 @@
       <c r="G226" t="s">
         <v>880</v>
       </c>
-      <c r="H226" s="10" t="s">
+      <c r="H226" s="5" t="s">
         <v>1015</v>
       </c>
-      <c r="I226" s="4" t="s">
+      <c r="I226" s="1" t="s">
         <v>1016</v>
       </c>
     </row>

</xml_diff>